<commit_message>
Added the fields from FMP to the excel
</commit_message>
<xml_diff>
--- a/profiles/ADBE/Financial analysis.xlsx
+++ b/profiles/ADBE/Financial analysis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\top kek\Desktop\Python\2_External APIs\profiles\ADBE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:11_{FDB18715-5BFB-48E9-84CD-25AC986DBE5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48F4142D-1E1A-4CBA-9F9B-342A21E4C5DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="24468" yWindow="-1308" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{9DC73D57-5531-4FDF-871C-B058328D7CA8}"/>
   </bookViews>
@@ -42,7 +42,7 @@
     <author>top kek</author>
   </authors>
   <commentList>
-    <comment ref="F31" authorId="0" shapeId="0" xr:uid="{7DBE328D-CFA5-4179-8126-719BDD5BF3EB}">
+    <comment ref="F52" authorId="0" shapeId="0" xr:uid="{7DBE328D-CFA5-4179-8126-719BDD5BF3EB}">
       <text>
         <r>
           <rPr>
@@ -93,7 +93,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="116">
   <si>
     <t>EURm</t>
   </si>
@@ -288,6 +288,159 @@
   </si>
   <si>
     <t>link</t>
+  </si>
+  <si>
+    <t>Source</t>
+  </si>
+  <si>
+    <t>IS</t>
+  </si>
+  <si>
+    <t>R&amp;D</t>
+  </si>
+  <si>
+    <t>SG&amp;A</t>
+  </si>
+  <si>
+    <t>interest</t>
+  </si>
+  <si>
+    <t>Field</t>
+  </si>
+  <si>
+    <t>cost of revenue</t>
+  </si>
+  <si>
+    <t>taxes</t>
+  </si>
+  <si>
+    <t>costOfRevenue</t>
+  </si>
+  <si>
+    <t>sellingGeneralAndAdministrativeExpenses</t>
+  </si>
+  <si>
+    <t>depreciationAndAmortization</t>
+  </si>
+  <si>
+    <t>researchAndDevelopmentExpenses</t>
+  </si>
+  <si>
+    <t>Support</t>
+  </si>
+  <si>
+    <t>interest income</t>
+  </si>
+  <si>
+    <t>interest expense</t>
+  </si>
+  <si>
+    <t>calcs</t>
+  </si>
+  <si>
+    <t>[internal]</t>
+  </si>
+  <si>
+    <t>incomeTaxExpense</t>
+  </si>
+  <si>
+    <t>interestIncome</t>
+  </si>
+  <si>
+    <t>interestExpense</t>
+  </si>
+  <si>
+    <t>inventory</t>
+  </si>
+  <si>
+    <t>BS</t>
+  </si>
+  <si>
+    <t>current  assets</t>
+  </si>
+  <si>
+    <t>current liabilities</t>
+  </si>
+  <si>
+    <t>totalCurrentAssets</t>
+  </si>
+  <si>
+    <t>totalCurrentLiabilities</t>
+  </si>
+  <si>
+    <t>change in WC</t>
+  </si>
+  <si>
+    <t>CF</t>
+  </si>
+  <si>
+    <t>changeInWorkingCapital</t>
+  </si>
+  <si>
+    <t>investmentsInPropertyPlantAndEquipment</t>
+  </si>
+  <si>
+    <t>commonStockRepurchased</t>
+  </si>
+  <si>
+    <t>buybacks</t>
+  </si>
+  <si>
+    <t>dividendsPaid</t>
+  </si>
+  <si>
+    <t>dividends</t>
+  </si>
+  <si>
+    <t>gross profit</t>
+  </si>
+  <si>
+    <t>receivables</t>
+  </si>
+  <si>
+    <t>payables</t>
+  </si>
+  <si>
+    <t>accountPayables</t>
+  </si>
+  <si>
+    <t>netReceivables</t>
+  </si>
+  <si>
+    <t>shortTermDebt</t>
+  </si>
+  <si>
+    <t>longTermDebt</t>
+  </si>
+  <si>
+    <t>capitalLeaseObligations</t>
+  </si>
+  <si>
+    <t>cashAndCashEquivalents</t>
+  </si>
+  <si>
+    <t>shortTermInvestments</t>
+  </si>
+  <si>
+    <t>cash</t>
+  </si>
+  <si>
+    <t>st investments</t>
+  </si>
+  <si>
+    <t>st debt</t>
+  </si>
+  <si>
+    <t>lt debt</t>
+  </si>
+  <si>
+    <t>leasing</t>
+  </si>
+  <si>
+    <t>EBITDA</t>
+  </si>
+  <si>
+    <t>net debt</t>
   </si>
 </sst>
 </file>
@@ -305,7 +458,7 @@
     <numFmt numFmtId="171" formatCode="\ dd\-mmm\-yy\ "/>
     <numFmt numFmtId="172" formatCode="\ #,##0\ \ ;\(#,##0\)\ ;\ \-\ ;\ @\ "/>
   </numFmts>
-  <fonts count="40" x14ac:knownFonts="1">
+  <fonts count="41" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF324150"/>
@@ -580,6 +733,12 @@
       <color indexed="81"/>
       <name val="Tahoma"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="2" tint="-9.9978637043366805E-2"/>
+      <name val="Consolas"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="51">
@@ -1141,7 +1300,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="54">
     <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1294,6 +1453,15 @@
     </xf>
     <xf numFmtId="172" fontId="34" fillId="0" borderId="15" xfId="52" applyNumberFormat="1" applyBorder="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="172" fontId="35" fillId="0" borderId="12" xfId="60" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="172" fontId="34" fillId="0" borderId="13" xfId="52" applyNumberFormat="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="172" fontId="40" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="62">
@@ -1776,7 +1944,7 @@
   <dimension ref="F4:R19"/>
   <sheetViews>
     <sheetView showGridLines="0" topLeftCell="D1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="R17" sqref="R17"/>
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -2155,10 +2323,10 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B3ED66B-4187-4A8D-853F-722DA914D9AA}">
   <sheetPr codeName="Sheet3"/>
-  <dimension ref="E5:Q38"/>
+  <dimension ref="E5:Q69"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A22" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G42" sqref="G42"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A46" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="F69" sqref="F69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -2223,249 +2391,680 @@
         <f t="shared" si="0"/>
         <v>2023</v>
       </c>
+      <c r="O7" s="45" t="s">
+        <v>65</v>
+      </c>
+      <c r="P7" s="52" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="8" spans="5:17" x14ac:dyDescent="0.25">
       <c r="F8" s="18" t="s">
         <v>38</v>
       </c>
+      <c r="O8" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="P8" s="11" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="9" spans="5:17" x14ac:dyDescent="0.25">
-      <c r="F9" s="46" t="s">
-        <v>39</v>
+      <c r="F9" s="18" t="s">
+        <v>71</v>
+      </c>
+      <c r="O9" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="P9" s="11" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="10" spans="5:17" x14ac:dyDescent="0.25">
       <c r="F10" s="46" t="s">
-        <v>40</v>
+        <v>68</v>
+      </c>
+      <c r="O10" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="P10" s="11" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="11" spans="5:17" x14ac:dyDescent="0.25">
       <c r="F11" s="46" t="s">
-        <v>41</v>
+        <v>39</v>
+      </c>
+      <c r="O11" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="P11" s="53" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="12" spans="5:17" x14ac:dyDescent="0.25">
       <c r="F12" s="46" t="s">
         <v>42</v>
       </c>
+      <c r="O12" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="P12" s="53" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="13" spans="5:17" x14ac:dyDescent="0.25">
       <c r="F13" s="46" t="s">
+        <v>40</v>
+      </c>
+      <c r="O13" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="P13" s="11" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="14" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="F14" s="46" t="s">
+        <v>41</v>
+      </c>
+      <c r="O14" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="P14" s="11" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="15" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="F15" s="46" t="s">
+        <v>67</v>
+      </c>
+      <c r="O15" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="P15" s="11" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="16" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="F16" s="46" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="14" spans="5:17" x14ac:dyDescent="0.25">
-      <c r="F14" s="46"/>
-    </row>
-    <row r="16" spans="5:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E16" s="47" t="s">
+      <c r="O16" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="P16" s="53" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="17" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="F17" s="46" t="s">
+        <v>69</v>
+      </c>
+      <c r="O17" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="P17" s="53" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="18" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="F18" s="46"/>
+    </row>
+    <row r="19" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="F19" s="51" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="20" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="F20" s="46" t="s">
+        <v>72</v>
+      </c>
+      <c r="O20" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="P20" s="11" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="21" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="F21" s="46" t="s">
+        <v>78</v>
+      </c>
+      <c r="O21" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="P21" s="11" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="22" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="F22" s="46" t="s">
+        <v>79</v>
+      </c>
+      <c r="O22" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="P22" s="11" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="23" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="F23" s="46" t="s">
+        <v>87</v>
+      </c>
+      <c r="O23" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="P23" s="11" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="24" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="F24" s="46" t="s">
+        <v>88</v>
+      </c>
+      <c r="O24" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="P24" s="11" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="25" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="F25" s="46" t="s">
+        <v>91</v>
+      </c>
+      <c r="O25" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="P25" s="11" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="26" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="F26" s="46" t="s">
+        <v>96</v>
+      </c>
+      <c r="O26" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="P26" s="11" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="27" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="F27" s="46" t="s">
+        <v>98</v>
+      </c>
+      <c r="O27" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="P27" s="11" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="28" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="F28" s="46"/>
+    </row>
+    <row r="30" spans="5:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E30" s="47" t="s">
         <v>44</v>
       </c>
-      <c r="F16" s="49" t="s">
+      <c r="F30" s="49" t="s">
         <v>45</v>
       </c>
-      <c r="G16" s="50"/>
-      <c r="H16" s="50"/>
-      <c r="I16" s="50"/>
-      <c r="J16" s="50"/>
-      <c r="K16" s="50"/>
-      <c r="L16" s="50"/>
-      <c r="M16" s="50"/>
-      <c r="N16" s="50"/>
-      <c r="O16" s="50"/>
-      <c r="P16" s="50"/>
-      <c r="Q16" s="50"/>
-    </row>
-    <row r="17" spans="5:17" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="18" spans="5:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F18" s="7" t="s">
+      <c r="G30" s="50"/>
+      <c r="H30" s="50"/>
+      <c r="I30" s="50"/>
+      <c r="J30" s="50"/>
+      <c r="K30" s="50"/>
+      <c r="L30" s="50"/>
+      <c r="M30" s="50"/>
+      <c r="N30" s="50"/>
+      <c r="O30" s="50"/>
+      <c r="P30" s="50"/>
+      <c r="Q30" s="50"/>
+    </row>
+    <row r="31" spans="5:17" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="32" spans="5:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F32" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="G18" s="45">
+      <c r="G32" s="45">
         <v>2017</v>
       </c>
-      <c r="H18" s="45">
-        <f>+G18+1</f>
+      <c r="H32" s="45">
+        <f>+G32+1</f>
         <v>2018</v>
       </c>
-      <c r="I18" s="45">
-        <f t="shared" ref="I18:M18" si="1">+H18+1</f>
+      <c r="I32" s="45">
+        <f t="shared" ref="I32:M32" si="1">+H32+1</f>
         <v>2019</v>
       </c>
-      <c r="J18" s="45">
+      <c r="J32" s="45">
         <f t="shared" si="1"/>
         <v>2020</v>
       </c>
-      <c r="K18" s="45">
+      <c r="K32" s="45">
         <f t="shared" si="1"/>
         <v>2021</v>
       </c>
-      <c r="L18" s="45">
+      <c r="L32" s="45">
         <f t="shared" si="1"/>
         <v>2022</v>
       </c>
-      <c r="M18" s="45">
+      <c r="M32" s="45">
         <f t="shared" si="1"/>
         <v>2023</v>
       </c>
-    </row>
-    <row r="19" spans="5:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F19" s="18" t="s">
+      <c r="O32" s="45" t="s">
+        <v>65</v>
+      </c>
+      <c r="P32" s="52" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="33" spans="6:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F33" s="18" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="20" spans="5:17" x14ac:dyDescent="0.25">
-      <c r="F20" s="18" t="s">
+      <c r="O33" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="P33" s="53" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="34" spans="6:16" x14ac:dyDescent="0.25">
+      <c r="F34" s="18" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="21" spans="5:17" x14ac:dyDescent="0.25">
-      <c r="F21" s="18" t="s">
+      <c r="O34" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="P34" s="53" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="35" spans="6:16" x14ac:dyDescent="0.25">
+      <c r="F35" s="18" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="22" spans="5:17" x14ac:dyDescent="0.25">
-      <c r="F22" s="18" t="s">
+      <c r="O35" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="P35" s="53" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="36" spans="6:16" x14ac:dyDescent="0.25">
+      <c r="F36" s="18" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="23" spans="5:17" x14ac:dyDescent="0.25">
-      <c r="F23" s="46"/>
-    </row>
-    <row r="24" spans="5:17" x14ac:dyDescent="0.25">
-      <c r="F24" s="7" t="s">
+      <c r="O36" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="P36" s="53" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="37" spans="6:16" x14ac:dyDescent="0.25">
+      <c r="F37" s="46"/>
+    </row>
+    <row r="38" spans="6:16" x14ac:dyDescent="0.25">
+      <c r="F38" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="G24" s="45">
+      <c r="G38" s="45">
         <v>2017</v>
       </c>
-      <c r="H24" s="45">
-        <f>+G24+1</f>
+      <c r="H38" s="45">
+        <f>+G38+1</f>
         <v>2018</v>
       </c>
-      <c r="I24" s="45">
-        <f t="shared" ref="I24:M24" si="2">+H24+1</f>
+      <c r="I38" s="45">
+        <f t="shared" ref="I38:M38" si="2">+H38+1</f>
         <v>2019</v>
       </c>
-      <c r="J24" s="45">
+      <c r="J38" s="45">
         <f t="shared" si="2"/>
         <v>2020</v>
       </c>
-      <c r="K24" s="45">
+      <c r="K38" s="45">
         <f t="shared" si="2"/>
         <v>2021</v>
       </c>
-      <c r="L24" s="45">
+      <c r="L38" s="45">
         <f t="shared" si="2"/>
         <v>2022</v>
       </c>
-      <c r="M24" s="45">
+      <c r="M38" s="45">
         <f t="shared" si="2"/>
         <v>2023</v>
       </c>
     </row>
-    <row r="25" spans="5:17" x14ac:dyDescent="0.25">
-      <c r="F25" s="18" t="s">
+    <row r="39" spans="6:16" x14ac:dyDescent="0.25">
+      <c r="F39" s="18" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="26" spans="5:17" x14ac:dyDescent="0.25">
-      <c r="F26" s="18" t="s">
+      <c r="O39" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="P39" s="53" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="40" spans="6:16" x14ac:dyDescent="0.25">
+      <c r="F40" s="18" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="27" spans="5:17" x14ac:dyDescent="0.25">
-      <c r="F27" s="18" t="s">
+      <c r="O40" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="P40" s="53" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="41" spans="6:16" x14ac:dyDescent="0.25">
+      <c r="F41" s="18" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="28" spans="5:17" x14ac:dyDescent="0.25">
-      <c r="F28" s="18" t="s">
+      <c r="O41" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="P41" s="53" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="42" spans="6:16" x14ac:dyDescent="0.25">
+      <c r="F42" s="18" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="31" spans="5:17" x14ac:dyDescent="0.25">
-      <c r="E31" s="47" t="s">
+      <c r="O42" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="P42" s="53" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="43" spans="6:16" x14ac:dyDescent="0.25">
+      <c r="F43" s="18"/>
+    </row>
+    <row r="44" spans="6:16" x14ac:dyDescent="0.25">
+      <c r="F44" s="51" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="45" spans="6:16" x14ac:dyDescent="0.25">
+      <c r="F45" s="18" t="s">
+        <v>99</v>
+      </c>
+      <c r="O45" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="P45" s="53" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="46" spans="6:16" x14ac:dyDescent="0.25">
+      <c r="F46" s="18" t="s">
+        <v>114</v>
+      </c>
+      <c r="O46" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="P46" s="53" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="47" spans="6:16" x14ac:dyDescent="0.25">
+      <c r="F47" s="18" t="s">
+        <v>100</v>
+      </c>
+      <c r="O47" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="P47" s="11" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="48" spans="6:16" x14ac:dyDescent="0.25">
+      <c r="F48" s="46" t="s">
+        <v>101</v>
+      </c>
+      <c r="O48" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="P48" s="11" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="49" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="F49" s="46" t="s">
+        <v>85</v>
+      </c>
+      <c r="O49" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="P49" s="11" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="50" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="F50" s="46"/>
+    </row>
+    <row r="52" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="E52" s="47" t="s">
         <v>56</v>
       </c>
-      <c r="F31" s="49" t="s">
+      <c r="F52" s="49" t="s">
         <v>57</v>
       </c>
-      <c r="G31" s="50"/>
-      <c r="H31" s="50"/>
-      <c r="I31" s="50"/>
-      <c r="J31" s="50"/>
-      <c r="K31" s="50"/>
-      <c r="L31" s="50"/>
-      <c r="M31" s="50"/>
-      <c r="N31" s="50"/>
-      <c r="O31" s="50"/>
-      <c r="P31" s="50"/>
-      <c r="Q31" s="50"/>
-    </row>
-    <row r="33" spans="6:13" x14ac:dyDescent="0.25">
-      <c r="F33" s="7" t="s">
+      <c r="G52" s="50"/>
+      <c r="H52" s="50"/>
+      <c r="I52" s="50"/>
+      <c r="J52" s="50"/>
+      <c r="K52" s="50"/>
+      <c r="L52" s="50"/>
+      <c r="M52" s="50"/>
+      <c r="N52" s="50"/>
+      <c r="O52" s="50"/>
+      <c r="P52" s="50"/>
+      <c r="Q52" s="50"/>
+    </row>
+    <row r="54" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="F54" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="G33" s="45">
+      <c r="G54" s="45">
         <v>2017</v>
       </c>
-      <c r="H33" s="45">
-        <f>+G33+1</f>
+      <c r="H54" s="45">
+        <f>+G54+1</f>
         <v>2018</v>
       </c>
-      <c r="I33" s="45">
-        <f t="shared" ref="I33:M33" si="3">+H33+1</f>
+      <c r="I54" s="45">
+        <f t="shared" ref="I54:M54" si="3">+H54+1</f>
         <v>2019</v>
       </c>
-      <c r="J33" s="45">
+      <c r="J54" s="45">
         <f t="shared" si="3"/>
         <v>2020</v>
       </c>
-      <c r="K33" s="45">
+      <c r="K54" s="45">
         <f t="shared" si="3"/>
         <v>2021</v>
       </c>
-      <c r="L33" s="45">
+      <c r="L54" s="45">
         <f t="shared" si="3"/>
         <v>2022</v>
       </c>
-      <c r="M33" s="45">
+      <c r="M54" s="45">
         <f t="shared" si="3"/>
         <v>2023</v>
       </c>
-    </row>
-    <row r="34" spans="6:13" x14ac:dyDescent="0.25">
-      <c r="F34" s="18" t="s">
+      <c r="O54" s="45" t="s">
+        <v>65</v>
+      </c>
+      <c r="P54" s="52" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="55" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="F55" s="18" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="35" spans="6:13" x14ac:dyDescent="0.25">
-      <c r="F35" s="18" t="s">
+      <c r="O55" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="P55" s="53" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="56" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="F56" s="18" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="36" spans="6:13" x14ac:dyDescent="0.25">
-      <c r="F36" s="18" t="s">
+      <c r="O56" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="P56" s="53" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="57" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="F57" s="18" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="37" spans="6:13" x14ac:dyDescent="0.25">
-      <c r="F37" s="18" t="s">
+      <c r="O57" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="P57" s="53" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="58" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="F58" s="18" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="38" spans="6:13" x14ac:dyDescent="0.25">
-      <c r="F38" s="46" t="s">
+      <c r="O58" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="P58" s="53" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="59" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="F59" s="46" t="s">
         <v>63</v>
       </c>
-      <c r="G38" s="48" t="s">
+      <c r="G59" s="48" t="s">
         <v>64</v>
+      </c>
+      <c r="O59" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="P59" s="53" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="61" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="F61" s="51" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="62" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="F62" s="18" t="s">
+        <v>109</v>
+      </c>
+      <c r="O62" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="P62" s="11" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="63" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="F63" s="46" t="s">
+        <v>110</v>
+      </c>
+      <c r="O63" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="P63" s="11" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="64" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="F64" s="46" t="s">
+        <v>111</v>
+      </c>
+      <c r="O64" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="P64" s="11" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="65" spans="6:16" x14ac:dyDescent="0.25">
+      <c r="F65" s="46" t="s">
+        <v>112</v>
+      </c>
+      <c r="O65" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="P65" s="11" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="66" spans="6:16" x14ac:dyDescent="0.25">
+      <c r="F66" s="46" t="s">
+        <v>113</v>
+      </c>
+      <c r="O66" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="P66" s="11" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="67" spans="6:16" x14ac:dyDescent="0.25">
+      <c r="F67" s="46" t="s">
+        <v>114</v>
+      </c>
+      <c r="O67" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="P67" s="53" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="68" spans="6:16" x14ac:dyDescent="0.25">
+      <c r="F68" s="46" t="s">
+        <v>79</v>
+      </c>
+      <c r="O68" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="P68" s="53" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="69" spans="6:16" x14ac:dyDescent="0.25">
+      <c r="F69" s="46" t="s">
+        <v>115</v>
+      </c>
+      <c r="O69" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="P69" s="53" t="s">
+        <v>81</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="G38" r:id="rId1" xr:uid="{04136F76-2C48-4215-8973-CCE83F77887B}"/>
+    <hyperlink ref="G59" r:id="rId1" xr:uid="{04136F76-2C48-4215-8973-CCE83F77887B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId2"/>

</xml_diff>

<commit_message>
Pulled the first analysis block
</commit_message>
<xml_diff>
--- a/profiles/ADBE/Financial analysis.xlsx
+++ b/profiles/ADBE/Financial analysis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\top kek\Desktop\Python\2_External APIs\profiles\ADBE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68CCBBB0-6908-4617-8595-4787EDCD5B68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DA1064A-C443-4786-A7B6-425F65276F2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="24468" yWindow="-1308" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{9DC73D57-5531-4FDF-871C-B058328D7CA8}"/>
   </bookViews>
@@ -16,7 +16,10 @@
     <sheet name="Intro" sheetId="2" r:id="rId1"/>
     <sheet name="Design" sheetId="1" r:id="rId2"/>
     <sheet name="Overview" sheetId="3" r:id="rId3"/>
-    <sheet name="0" sheetId="4" r:id="rId4"/>
+    <sheet name="BS" sheetId="5" r:id="rId4"/>
+    <sheet name="IS" sheetId="6" r:id="rId5"/>
+    <sheet name="CF" sheetId="7" r:id="rId6"/>
+    <sheet name="0" sheetId="4" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -93,7 +96,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372" uniqueCount="213">
   <si>
     <t>EURm</t>
   </si>
@@ -441,6 +444,297 @@
   </si>
   <si>
     <t>net debt</t>
+  </si>
+  <si>
+    <t>symbol</t>
+  </si>
+  <si>
+    <t>reportedCurrency</t>
+  </si>
+  <si>
+    <t>cik</t>
+  </si>
+  <si>
+    <t>fillingDate</t>
+  </si>
+  <si>
+    <t>acceptedDate</t>
+  </si>
+  <si>
+    <t>calendarYear</t>
+  </si>
+  <si>
+    <t>period</t>
+  </si>
+  <si>
+    <t>cashAndShortTermInvestments</t>
+  </si>
+  <si>
+    <t>otherCurrentAssets</t>
+  </si>
+  <si>
+    <t>propertyPlantEquipmentNet</t>
+  </si>
+  <si>
+    <t>goodwill</t>
+  </si>
+  <si>
+    <t>intangibleAssets</t>
+  </si>
+  <si>
+    <t>goodwillAndIntangibleAssets</t>
+  </si>
+  <si>
+    <t>longTermInvestments</t>
+  </si>
+  <si>
+    <t>taxAssets</t>
+  </si>
+  <si>
+    <t>otherNonCurrentAssets</t>
+  </si>
+  <si>
+    <t>totalNonCurrentAssets</t>
+  </si>
+  <si>
+    <t>otherAssets</t>
+  </si>
+  <si>
+    <t>totalAssets</t>
+  </si>
+  <si>
+    <t>taxPayables</t>
+  </si>
+  <si>
+    <t>deferredRevenue</t>
+  </si>
+  <si>
+    <t>otherCurrentLiabilities</t>
+  </si>
+  <si>
+    <t>deferredRevenueNonCurrent</t>
+  </si>
+  <si>
+    <t>deferredTaxLiabilitiesNonCurrent</t>
+  </si>
+  <si>
+    <t>otherNonCurrentLiabilities</t>
+  </si>
+  <si>
+    <t>totalNonCurrentLiabilities</t>
+  </si>
+  <si>
+    <t>otherLiabilities</t>
+  </si>
+  <si>
+    <t>totalLiabilities</t>
+  </si>
+  <si>
+    <t>preferredStock</t>
+  </si>
+  <si>
+    <t>commonStock</t>
+  </si>
+  <si>
+    <t>retainedEarnings</t>
+  </si>
+  <si>
+    <t>accumulatedOtherComprehensiveIncomeLoss</t>
+  </si>
+  <si>
+    <t>othertotalStockholdersEquity</t>
+  </si>
+  <si>
+    <t>totalStockholdersEquity</t>
+  </si>
+  <si>
+    <t>totalEquity</t>
+  </si>
+  <si>
+    <t>totalLiabilitiesAndStockholdersEquity</t>
+  </si>
+  <si>
+    <t>minorityInterest</t>
+  </si>
+  <si>
+    <t>totalLiabilitiesAndTotalEquity</t>
+  </si>
+  <si>
+    <t>totalInvestments</t>
+  </si>
+  <si>
+    <t>totalDebt</t>
+  </si>
+  <si>
+    <t>netDebt</t>
+  </si>
+  <si>
+    <t>finalLink</t>
+  </si>
+  <si>
+    <t>Column</t>
+  </si>
+  <si>
+    <t>Example</t>
+  </si>
+  <si>
+    <t>2023-12-01</t>
+  </si>
+  <si>
+    <t>ADBE</t>
+  </si>
+  <si>
+    <t>USD</t>
+  </si>
+  <si>
+    <t>0000796343</t>
+  </si>
+  <si>
+    <t>2024-01-17</t>
+  </si>
+  <si>
+    <t>2024-01-16 20:01:55</t>
+  </si>
+  <si>
+    <t>2023</t>
+  </si>
+  <si>
+    <t>FY</t>
+  </si>
+  <si>
+    <t>https://www.sec.gov/Archives/edgar/data/796343/000079634324000006/0000796343-24-000006-index.htm</t>
+  </si>
+  <si>
+    <t>https://www.sec.gov/Archives/edgar/data/796343/000079634324000006/adbe-20231201.htm</t>
+  </si>
+  <si>
+    <t>grossProfit</t>
+  </si>
+  <si>
+    <t>grossProfitRatio</t>
+  </si>
+  <si>
+    <t>generalAndAdministrativeExpenses</t>
+  </si>
+  <si>
+    <t>sellingAndMarketingExpenses</t>
+  </si>
+  <si>
+    <t>otherExpenses</t>
+  </si>
+  <si>
+    <t>operatingExpenses</t>
+  </si>
+  <si>
+    <t>costAndExpenses</t>
+  </si>
+  <si>
+    <t>ebitda</t>
+  </si>
+  <si>
+    <t>ebitdaratio</t>
+  </si>
+  <si>
+    <t>operatingIncome</t>
+  </si>
+  <si>
+    <t>operatingIncomeRatio</t>
+  </si>
+  <si>
+    <t>totalOtherIncomeExpensesNet</t>
+  </si>
+  <si>
+    <t>incomeBeforeTax</t>
+  </si>
+  <si>
+    <t>incomeBeforeTaxRatio</t>
+  </si>
+  <si>
+    <t>netIncome</t>
+  </si>
+  <si>
+    <t>netIncomeRatio</t>
+  </si>
+  <si>
+    <t>eps</t>
+  </si>
+  <si>
+    <t>epsdiluted</t>
+  </si>
+  <si>
+    <t>weightedAverageShsOut</t>
+  </si>
+  <si>
+    <t>weightedAverageShsOutDil</t>
+  </si>
+  <si>
+    <t>deferredIncomeTax</t>
+  </si>
+  <si>
+    <t>stockBasedCompensation</t>
+  </si>
+  <si>
+    <t>accountsReceivables</t>
+  </si>
+  <si>
+    <t>accountsPayables</t>
+  </si>
+  <si>
+    <t>otherWorkingCapital</t>
+  </si>
+  <si>
+    <t>otherNonCashItems</t>
+  </si>
+  <si>
+    <t>netCashProvidedByOperatingActivities</t>
+  </si>
+  <si>
+    <t>acquisitionsNet</t>
+  </si>
+  <si>
+    <t>purchasesOfInvestments</t>
+  </si>
+  <si>
+    <t>salesMaturitiesOfInvestments</t>
+  </si>
+  <si>
+    <t>otherInvestingActivites</t>
+  </si>
+  <si>
+    <t>netCashUsedForInvestingActivites</t>
+  </si>
+  <si>
+    <t>debtRepayment</t>
+  </si>
+  <si>
+    <t>commonStockIssued</t>
+  </si>
+  <si>
+    <t>otherFinancingActivites</t>
+  </si>
+  <si>
+    <t>netCashUsedProvidedByFinancingActivities</t>
+  </si>
+  <si>
+    <t>effectOfForexChangesOnCash</t>
+  </si>
+  <si>
+    <t>netChangeInCash</t>
+  </si>
+  <si>
+    <t>cashAtEndOfPeriod</t>
+  </si>
+  <si>
+    <t>cashAtBeginningOfPeriod</t>
+  </si>
+  <si>
+    <t>operatingCashFlow</t>
+  </si>
+  <si>
+    <t>capitalExpenditure</t>
+  </si>
+  <si>
+    <t>freeCashFlow</t>
   </si>
 </sst>
 </file>
@@ -1300,7 +1594,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="56">
     <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1463,6 +1757,8 @@
     <xf numFmtId="172" fontId="40" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="172" fontId="37" fillId="0" borderId="0" xfId="61" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="62">
     <cellStyle name="20% - Accent1" xfId="24" builtinId="30" hidden="1"/>
@@ -2326,7 +2622,7 @@
   <dimension ref="E5:Q69"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -3073,6 +3369,1269 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB68C096-070C-490A-8EBF-7569BB73525B}">
+  <dimension ref="F5:H59"/>
+  <sheetViews>
+    <sheetView showGridLines="0" zoomScale="115" zoomScaleNormal="115" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="5" width="3.77734375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="42.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="11" width="14.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="3.77734375" style="1" customWidth="1"/>
+    <col min="13" max="13" width="28.44140625" style="1" customWidth="1"/>
+    <col min="14" max="14" width="3.77734375" style="1" customWidth="1"/>
+    <col min="15" max="15" width="13.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="18" width="10.77734375" style="1" customWidth="1"/>
+    <col min="19" max="16384" width="9.21875" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="5" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F5" s="52" t="s">
+        <v>158</v>
+      </c>
+      <c r="G5" s="52" t="s">
+        <v>159</v>
+      </c>
+      <c r="H5" s="52"/>
+    </row>
+    <row r="6" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G6" s="54" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="7" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F7" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="G7" s="54" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="8" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F8" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="G8" s="54" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="9" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F9" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="G9" s="54" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="10" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F10" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="G10" s="54" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="11" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F11" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="G11" s="54" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="12" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F12" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="G12" s="54" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="13" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F13" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="G13" s="54" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="14" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F14" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="G14" s="54">
+        <v>7141000000</v>
+      </c>
+    </row>
+    <row r="15" spans="6:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F15" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="G15" s="54">
+        <v>701000000</v>
+      </c>
+    </row>
+    <row r="16" spans="6:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F16" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="G16" s="54">
+        <v>7842000000</v>
+      </c>
+    </row>
+    <row r="17" spans="6:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F17" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="G17" s="54">
+        <v>2224000000</v>
+      </c>
+    </row>
+    <row r="18" spans="6:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F18" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="G18" s="54">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F19" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="G19" s="54">
+        <v>1018000000</v>
+      </c>
+    </row>
+    <row r="20" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F20" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="G20" s="54">
+        <v>11084000000</v>
+      </c>
+    </row>
+    <row r="21" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F21" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="G21" s="54">
+        <v>2388000000</v>
+      </c>
+    </row>
+    <row r="22" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F22" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="G22" s="54">
+        <v>12805000000</v>
+      </c>
+    </row>
+    <row r="23" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F23" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="G23" s="54">
+        <v>1088000000</v>
+      </c>
+    </row>
+    <row r="24" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F24" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="G24" s="54">
+        <v>13893000000</v>
+      </c>
+    </row>
+    <row r="25" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F25" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="G25" s="54">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F26" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="G26" s="54">
+        <v>1191000000</v>
+      </c>
+    </row>
+    <row r="27" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F27" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="G27" s="54">
+        <v>1223000000</v>
+      </c>
+    </row>
+    <row r="28" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F28" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="G28" s="54">
+        <v>18695000000</v>
+      </c>
+    </row>
+    <row r="29" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F29" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="G29" s="54">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F30" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="G30" s="54">
+        <v>29779000000</v>
+      </c>
+    </row>
+    <row r="31" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F31" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="G31" s="54">
+        <v>314000000</v>
+      </c>
+    </row>
+    <row r="32" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F32" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="G32" s="54">
+        <v>73000000</v>
+      </c>
+    </row>
+    <row r="33" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F33" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="G33" s="54">
+        <v>85000000</v>
+      </c>
+    </row>
+    <row r="34" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F34" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="G34" s="54">
+        <v>5837000000</v>
+      </c>
+    </row>
+    <row r="35" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F35" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="G35" s="54">
+        <v>2027000000</v>
+      </c>
+    </row>
+    <row r="36" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F36" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="G36" s="54">
+        <v>8251000000</v>
+      </c>
+    </row>
+    <row r="37" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F37" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="G37" s="54">
+        <v>4007000000</v>
+      </c>
+    </row>
+    <row r="38" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F38" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="G38" s="54">
+        <v>113000000</v>
+      </c>
+    </row>
+    <row r="39" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F39" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="G39" s="54">
+        <v>514000000</v>
+      </c>
+    </row>
+    <row r="40" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F40" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="G40" s="54">
+        <v>376000000</v>
+      </c>
+    </row>
+    <row r="41" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F41" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="G41" s="54">
+        <v>5010000000</v>
+      </c>
+    </row>
+    <row r="42" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F42" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="G42" s="54">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F43" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="G43" s="54">
+        <v>446000000</v>
+      </c>
+    </row>
+    <row r="44" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F44" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="G44" s="54">
+        <v>13261000000</v>
+      </c>
+    </row>
+    <row r="45" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F45" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="G45" s="54">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F46" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="G46" s="54">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F47" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="G47" s="54">
+        <v>33346000000</v>
+      </c>
+    </row>
+    <row r="48" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F48" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="G48" s="54">
+        <v>-285000000</v>
+      </c>
+    </row>
+    <row r="49" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F49" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="G49" s="54">
+        <v>-16543000000</v>
+      </c>
+    </row>
+    <row r="50" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F50" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="G50" s="54">
+        <v>16518000000</v>
+      </c>
+    </row>
+    <row r="51" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F51" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="G51" s="54">
+        <v>16518000000</v>
+      </c>
+    </row>
+    <row r="52" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F52" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="G52" s="54">
+        <v>29779000000</v>
+      </c>
+    </row>
+    <row r="53" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F53" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="G53" s="54">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F54" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="G54" s="54">
+        <v>29779000000</v>
+      </c>
+    </row>
+    <row r="55" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F55" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="G55" s="54">
+        <v>701000000</v>
+      </c>
+    </row>
+    <row r="56" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F56" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="G56" s="54">
+        <v>4080000000</v>
+      </c>
+    </row>
+    <row r="57" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F57" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="G57" s="54">
+        <v>-3061000000</v>
+      </c>
+    </row>
+    <row r="58" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F58" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="G58" s="55" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="59" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F59" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="G59" s="55" t="s">
+        <v>169</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="G58" r:id="rId1" xr:uid="{68DB25E7-FC3D-4099-BAE2-CD17BD7491EB}"/>
+    <hyperlink ref="G59" r:id="rId2" xr:uid="{85321FB0-AB00-4EA0-905B-7F3DDEB41509}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95B6F0F8-3D00-4E0E-AF03-B4DF548B5411}">
+  <dimension ref="F5:H59"/>
+  <sheetViews>
+    <sheetView showGridLines="0" zoomScale="115" zoomScaleNormal="115" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="5" width="3.77734375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="42.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="11" width="14.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="3.77734375" style="1" customWidth="1"/>
+    <col min="13" max="13" width="28.44140625" style="1" customWidth="1"/>
+    <col min="14" max="14" width="3.77734375" style="1" customWidth="1"/>
+    <col min="15" max="15" width="13.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="18" width="10.77734375" style="1" customWidth="1"/>
+    <col min="19" max="16384" width="9.21875" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="5" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F5" s="52" t="s">
+        <v>158</v>
+      </c>
+      <c r="G5" s="52" t="s">
+        <v>159</v>
+      </c>
+      <c r="H5" s="52"/>
+    </row>
+    <row r="6" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G6" s="54" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="7" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F7" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="G7" s="54" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="8" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F8" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="G8" s="54" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="9" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F9" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="G9" s="54" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="10" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F10" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="G10" s="54" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="11" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F11" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="G11" s="54" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="12" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F12" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="G12" s="54" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="13" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F13" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="G13" s="54" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="14" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F14" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="G14" s="54">
+        <v>19409000000</v>
+      </c>
+    </row>
+    <row r="15" spans="6:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F15" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="G15" s="54">
+        <v>2354000000</v>
+      </c>
+    </row>
+    <row r="16" spans="6:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F16" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="G16" s="54">
+        <v>17055000000</v>
+      </c>
+    </row>
+    <row r="17" spans="6:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F17" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="G17" s="54">
+        <v>0.87871605959999999</v>
+      </c>
+    </row>
+    <row r="18" spans="6:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F18" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="G18" s="54">
+        <v>3473000000</v>
+      </c>
+    </row>
+    <row r="19" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F19" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="G19" s="54">
+        <v>1413000000</v>
+      </c>
+    </row>
+    <row r="20" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F20" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="G20" s="54">
+        <v>5351000000</v>
+      </c>
+    </row>
+    <row r="21" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F21" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="G21" s="54">
+        <v>6764000000</v>
+      </c>
+    </row>
+    <row r="22" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F22" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="G22" s="54">
+        <v>246000000</v>
+      </c>
+    </row>
+    <row r="23" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F23" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="G23" s="54">
+        <v>10405000000</v>
+      </c>
+    </row>
+    <row r="24" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F24" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="G24" s="54">
+        <v>12759000000</v>
+      </c>
+    </row>
+    <row r="25" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F25" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="G25" s="54">
+        <v>269000000</v>
+      </c>
+    </row>
+    <row r="26" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F26" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="G26" s="54">
+        <v>113000000</v>
+      </c>
+    </row>
+    <row r="27" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F27" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="G27" s="54">
+        <v>944000000</v>
+      </c>
+    </row>
+    <row r="28" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F28" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="G28" s="54">
+        <v>7768000000</v>
+      </c>
+    </row>
+    <row r="29" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F29" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="G29" s="54">
+        <v>0.40022669900000002</v>
+      </c>
+    </row>
+    <row r="30" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F30" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="G30" s="54">
+        <v>6650000000</v>
+      </c>
+    </row>
+    <row r="31" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F31" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="G31" s="54">
+        <v>0.34262455559999999</v>
+      </c>
+    </row>
+    <row r="32" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F32" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="G32" s="54">
+        <v>262000000</v>
+      </c>
+    </row>
+    <row r="33" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F33" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="G33" s="54">
+        <v>6799000000</v>
+      </c>
+    </row>
+    <row r="34" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F34" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="G34" s="54">
+        <v>0.35030140659999998</v>
+      </c>
+    </row>
+    <row r="35" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F35" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="G35" s="54">
+        <v>1371000000</v>
+      </c>
+    </row>
+    <row r="36" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F36" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="G36" s="54">
+        <v>5428000000</v>
+      </c>
+    </row>
+    <row r="37" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F37" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="G37" s="54">
+        <v>0.27966407339999999</v>
+      </c>
+    </row>
+    <row r="38" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F38" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="G38" s="54">
+        <v>11.93</v>
+      </c>
+    </row>
+    <row r="39" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F39" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="G39" s="54">
+        <v>11.83</v>
+      </c>
+    </row>
+    <row r="40" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F40" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="G40" s="54">
+        <v>457000000</v>
+      </c>
+    </row>
+    <row r="41" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F41" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="G41" s="54">
+        <v>459000000</v>
+      </c>
+    </row>
+    <row r="42" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F42" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="G42" s="55" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="43" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F43" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="G43" s="55" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="44" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="G44" s="54"/>
+    </row>
+    <row r="45" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="G45" s="54"/>
+    </row>
+    <row r="46" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="G46" s="54"/>
+    </row>
+    <row r="47" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="G47" s="54"/>
+    </row>
+    <row r="48" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="G48" s="54"/>
+    </row>
+    <row r="49" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G49" s="54"/>
+    </row>
+    <row r="50" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G50" s="54"/>
+    </row>
+    <row r="51" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G51" s="54"/>
+    </row>
+    <row r="52" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G52" s="54"/>
+    </row>
+    <row r="53" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G53" s="54"/>
+    </row>
+    <row r="54" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G54" s="54"/>
+    </row>
+    <row r="55" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G55" s="54"/>
+    </row>
+    <row r="56" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G56" s="54"/>
+    </row>
+    <row r="57" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G57" s="54"/>
+    </row>
+    <row r="58" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G58" s="55"/>
+    </row>
+    <row r="59" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G59" s="55"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="G42" r:id="rId1" xr:uid="{F6D1583B-1791-43F8-8706-23BB20909443}"/>
+    <hyperlink ref="G43" r:id="rId2" xr:uid="{461972E0-03EA-4A6C-8B32-DC6601898EF6}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07536025-EEFB-47B0-9BFC-0CD5458496B3}">
+  <dimension ref="F5:H59"/>
+  <sheetViews>
+    <sheetView showGridLines="0" zoomScale="115" zoomScaleNormal="115" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="5" width="3.77734375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="42.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="11" width="14.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="3.77734375" style="1" customWidth="1"/>
+    <col min="13" max="13" width="28.44140625" style="1" customWidth="1"/>
+    <col min="14" max="14" width="3.77734375" style="1" customWidth="1"/>
+    <col min="15" max="15" width="13.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="18" width="10.77734375" style="1" customWidth="1"/>
+    <col min="19" max="16384" width="9.21875" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="5" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F5" s="52" t="s">
+        <v>158</v>
+      </c>
+      <c r="G5" s="52" t="s">
+        <v>159</v>
+      </c>
+      <c r="H5" s="52"/>
+    </row>
+    <row r="6" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G6" s="54" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="7" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F7" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="G7" s="54" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="8" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F8" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="G8" s="54" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="9" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F9" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="G9" s="54" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="10" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F10" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="G10" s="54" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="11" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F11" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="G11" s="54" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="12" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F12" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="G12" s="54" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="13" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F13" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="G13" s="54" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="14" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F14" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="G14" s="54">
+        <v>5428000000</v>
+      </c>
+    </row>
+    <row r="15" spans="6:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F15" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="G15" s="54">
+        <v>872000000</v>
+      </c>
+    </row>
+    <row r="16" spans="6:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F16" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="G16" s="54">
+        <v>-426000000</v>
+      </c>
+    </row>
+    <row r="17" spans="6:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F17" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="G17" s="54">
+        <v>1718000000</v>
+      </c>
+    </row>
+    <row r="18" spans="6:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F18" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="G18" s="54">
+        <v>-355000000</v>
+      </c>
+    </row>
+    <row r="19" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F19" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="G19" s="54">
+        <v>-159000000</v>
+      </c>
+    </row>
+    <row r="20" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F20" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="G20" s="54">
+        <v>208000000</v>
+      </c>
+    </row>
+    <row r="21" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F21" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="G21" s="54">
+        <v>-49000000</v>
+      </c>
+    </row>
+    <row r="22" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F22" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="G22" s="54">
+        <v>-355000000</v>
+      </c>
+    </row>
+    <row r="23" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F23" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="G23" s="54">
+        <v>65000000</v>
+      </c>
+    </row>
+    <row r="24" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F24" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="G24" s="54">
+        <v>7302000000</v>
+      </c>
+    </row>
+    <row r="25" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F25" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="G25" s="54">
+        <v>-360000000</v>
+      </c>
+    </row>
+    <row r="26" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F26" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="G26" s="54">
+        <v>-1136000000</v>
+      </c>
+    </row>
+    <row r="27" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F27" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="G27" s="54">
+        <v>-53000000</v>
+      </c>
+    </row>
+    <row r="28" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F28" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="G28" s="54">
+        <v>1189000000</v>
+      </c>
+    </row>
+    <row r="29" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F29" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="G29" s="54">
+        <v>1136000000</v>
+      </c>
+    </row>
+    <row r="30" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F30" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="G30" s="54">
+        <v>776000000</v>
+      </c>
+    </row>
+    <row r="31" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F31" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="G31" s="54">
+        <v>-500000000</v>
+      </c>
+    </row>
+    <row r="32" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F32" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="G32" s="54">
+        <v>314000000</v>
+      </c>
+    </row>
+    <row r="33" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F33" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="G33" s="54">
+        <v>-4400000000</v>
+      </c>
+    </row>
+    <row r="34" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F34" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="G34" s="54">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F35" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="G35" s="54">
+        <v>-596000000</v>
+      </c>
+    </row>
+    <row r="36" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F36" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="G36" s="54">
+        <v>-5182000000</v>
+      </c>
+    </row>
+    <row r="37" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F37" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="G37" s="54">
+        <v>9000000</v>
+      </c>
+    </row>
+    <row r="38" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F38" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="G38" s="54">
+        <v>2905000000</v>
+      </c>
+    </row>
+    <row r="39" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F39" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="G39" s="54">
+        <v>7141000000</v>
+      </c>
+    </row>
+    <row r="40" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F40" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="G40" s="54">
+        <v>4236000000</v>
+      </c>
+    </row>
+    <row r="41" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F41" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="G41" s="54">
+        <v>7302000000</v>
+      </c>
+    </row>
+    <row r="42" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F42" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="G42" s="54">
+        <v>-360000000</v>
+      </c>
+    </row>
+    <row r="43" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F43" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="G43" s="54">
+        <v>6942000000</v>
+      </c>
+    </row>
+    <row r="44" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F44" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="G44" s="55" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="45" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F45" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="G45" s="55" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="46" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="G46" s="54"/>
+    </row>
+    <row r="47" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="G47" s="54"/>
+    </row>
+    <row r="48" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="G48" s="54"/>
+    </row>
+    <row r="49" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G49" s="54"/>
+    </row>
+    <row r="50" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G50" s="54"/>
+    </row>
+    <row r="51" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G51" s="54"/>
+    </row>
+    <row r="52" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G52" s="54"/>
+    </row>
+    <row r="53" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G53" s="54"/>
+    </row>
+    <row r="54" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G54" s="54"/>
+    </row>
+    <row r="55" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G55" s="54"/>
+    </row>
+    <row r="56" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G56" s="54"/>
+    </row>
+    <row r="57" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G57" s="54"/>
+    </row>
+    <row r="58" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G58" s="55"/>
+    </row>
+    <row r="59" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G59" s="55"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="G44" r:id="rId1" xr:uid="{E4BFBB07-9186-4A60-9CF1-57746BEE8BD0}"/>
+    <hyperlink ref="G45" r:id="rId2" xr:uid="{FC73A6E7-4CFE-4870-81B4-E1469201A5A9}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE9AB1EF-E2E2-4B80-84CC-527727B171CC}">
   <dimension ref="F5:F18"/>
   <sheetViews>

</xml_diff>